<commit_message>
Allow second naming convention
</commit_message>
<xml_diff>
--- a/mock_metadata.xlsx
+++ b/mock_metadata.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,50 +461,60 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>FLT3</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>mock_col_0</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>mock_col_1</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>mock_col_2</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>mock_col_3</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>mock_col_4</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>mock_col_5</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>mock_col_6</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>mock_col_7</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>mock_col_8</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>mock_col_9</t>
         </is>
@@ -512,10 +522,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>901153000</v>
+        <v>108731871</v>
       </c>
       <c r="B2" t="n">
-        <v>59797212</v>
+        <v>91890481</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -524,53 +534,67 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Marie</t>
+          <t>MARIE</t>
         </is>
       </c>
       <c r="E2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>WT</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>CZSBV11530005</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>9.766997666981421</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>8</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>2.935015581362097</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>0.8544073566273735</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>2.9784009061862315</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>7.288273572721245</t>
+        </is>
+      </c>
+      <c r="O2" t="n">
+        <v>6.554225855557608</v>
+      </c>
+      <c r="P2" t="n">
         <v>1</v>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>9.766997666981421</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>8</v>
-      </c>
-      <c r="I2" t="n">
-        <v>2</v>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>0.8544073566273735</t>
-        </is>
-      </c>
-      <c r="K2" t="n">
-        <v>2.978400906186232</v>
-      </c>
-      <c r="L2" t="n">
-        <v>7.288273572721245</v>
-      </c>
-      <c r="M2" t="n">
-        <v>6.554225855557608</v>
-      </c>
-      <c r="N2" t="n">
-        <v>1.220804415290607</v>
-      </c>
-      <c r="O2" t="n">
+      <c r="Q2" t="n">
         <v>8.579403861447053</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>871918904</v>
+        <v>183205182</v>
       </c>
       <c r="B3" t="n">
-        <v>81475433</v>
+        <v>47064024</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -579,108 +603,136 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Jean</t>
+          <t>JEAN</t>
         </is>
       </c>
       <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>WT</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>UGOQV08105276</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>3.801957350196178</v>
+      </c>
+      <c r="I3" t="n">
+        <v>6</v>
+      </c>
+      <c r="J3" t="n">
         <v>2</v>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>3.8019573501961776</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>6</v>
-      </c>
-      <c r="H3" t="n">
-        <v>2</v>
-      </c>
-      <c r="I3" t="n">
-        <v>7</v>
-      </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>7.333144993171773</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
         <is>
           <t>2.2016043728738346</t>
         </is>
       </c>
-      <c r="K3" t="n">
-        <v>6.19161016367253</v>
-      </c>
-      <c r="L3" t="n">
-        <v>1.755449978176405</v>
-      </c>
-      <c r="M3" t="n">
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>6.19161016367253</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>1.7554499781764055</t>
+        </is>
+      </c>
+      <c r="O3" t="n">
         <v>9.106845690724835</v>
       </c>
-      <c r="N3" t="n">
-        <v>5.311501483237562</v>
-      </c>
-      <c r="O3" t="n">
+      <c r="P3" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q3" t="n">
         <v>7.024108748899226</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>276201972</v>
+        <v>266181764</v>
       </c>
       <c r="B4" t="n">
-        <v>18320518</v>
+        <v>35129425</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>bernard</t>
+          <t>BERNARD</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>sophie</t>
+          <t>Sophie</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>9.232462337639554</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
+          <t>TKD</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>SMYLP59770792</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>9.232462337639554</v>
+      </c>
+      <c r="I4" t="n">
         <v>6</v>
       </c>
-      <c r="H4" t="n">
+      <c r="J4" t="n">
         <v>8</v>
       </c>
-      <c r="I4" t="n">
-        <v>8</v>
-      </c>
-      <c r="J4" t="inlineStr">
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>8.088307025622912</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
         <is>
           <t>6.8117600564649585</t>
         </is>
       </c>
-      <c r="K4" t="n">
-        <v>3.017574296201845</v>
-      </c>
-      <c r="L4" t="n">
-        <v>6.927590935814957</v>
-      </c>
-      <c r="M4" t="n">
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>3.017574296201845</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>6.9275909358149566</t>
+        </is>
+      </c>
+      <c r="O4" t="n">
         <v>1.525846598449274</v>
       </c>
-      <c r="N4" t="n">
-        <v>9.131380419328305</v>
-      </c>
-      <c r="O4" t="n">
+      <c r="P4" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q4" t="n">
         <v>5.686140286219992</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>402424270</v>
+        <v>378353862</v>
       </c>
       <c r="B5" t="n">
-        <v>96575977</v>
+        <v>93405827</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -693,58 +745,72 @@
         </is>
       </c>
       <c r="E5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>WT</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>GBJZB38154719</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>2.616924238635442</v>
+      </c>
+      <c r="I5" t="n">
+        <v>6</v>
+      </c>
+      <c r="J5" t="n">
+        <v>9</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>8.870869741717364</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>1.3441008942863109</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>1.7484645112507746</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>0.9283302374194224</t>
+        </is>
+      </c>
+      <c r="O5" t="n">
+        <v>5.886323190849075</v>
+      </c>
+      <c r="P5" t="n">
         <v>1</v>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2.616924238635442</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>6</v>
-      </c>
-      <c r="H5" t="n">
-        <v>9</v>
-      </c>
-      <c r="I5" t="n">
-        <v>8</v>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>1.3441008942863109</t>
-        </is>
-      </c>
-      <c r="K5" t="n">
-        <v>1.748464511250775</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.9283302374194224</v>
-      </c>
-      <c r="M5" t="n">
-        <v>5.886323190849075</v>
-      </c>
-      <c r="N5" t="n">
-        <v>1.824672702715892</v>
-      </c>
-      <c r="O5" t="n">
+      <c r="Q5" t="n">
         <v>9.810992114290196</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>441266181</v>
+        <v>846592814</v>
       </c>
       <c r="B6" t="n">
-        <v>76435129</v>
+        <v>46694816</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Petit</t>
+          <t>petit</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Lucas</t>
+          <t>lucas</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -752,45 +818,59 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>3.1909705841419758</t>
-        </is>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
+          <t>ITD</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>TFERC52001230</t>
+        </is>
       </c>
       <c r="H6" t="n">
-        <v>8</v>
+        <v>3.190970584141976</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="J6" t="n">
+        <v>8</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>0.24833211267027866</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
         <is>
           <t>9.565136908680433</t>
         </is>
       </c>
-      <c r="K6" t="n">
-        <v>4.95505195217647</v>
-      </c>
-      <c r="L6" t="n">
-        <v>5.564015705845731</v>
-      </c>
-      <c r="M6" t="n">
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>4.95505195217647</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>5.564015705845731</t>
+        </is>
+      </c>
+      <c r="O6" t="n">
         <v>5.037655996150194</v>
       </c>
-      <c r="N6" t="n">
-        <v>9.914987103933043</v>
-      </c>
-      <c r="O6" t="n">
+      <c r="P6" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q6" t="n">
         <v>0.9035270116837701</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>163040381</v>
+        <v>495953289</v>
       </c>
       <c r="B7" t="n">
-        <v>54719416</v>
+        <v>77071057</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -799,7 +879,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>PAUL</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -807,45 +887,59 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>1.1809123296664281</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
+          <t>ITD</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>LOHYP26401764</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>1.180912329666428</v>
+      </c>
+      <c r="I7" t="n">
         <v>9</v>
       </c>
-      <c r="H7" t="n">
+      <c r="J7" t="n">
         <v>4</v>
       </c>
-      <c r="I7" t="n">
-        <v>5</v>
-      </c>
-      <c r="J7" t="inlineStr">
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>5.125494476917045</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
         <is>
           <t>1.3652397740514988</t>
         </is>
       </c>
-      <c r="K7" t="n">
-        <v>7.605704002660505</v>
-      </c>
-      <c r="L7" t="n">
-        <v>1.024941347304994</v>
-      </c>
-      <c r="M7" t="n">
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>7.605704002660505</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>1.024941347304994</t>
+        </is>
+      </c>
+      <c r="O7" t="n">
         <v>1.738089819802944</v>
       </c>
-      <c r="N7" t="n">
-        <v>8.799048899254057</v>
-      </c>
-      <c r="O7" t="n">
+      <c r="P7" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q7" t="n">
         <v>7.270797710217943</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>835386293</v>
+        <v>418998134</v>
       </c>
       <c r="B8" t="n">
-        <v>40582787</v>
+        <v>52060032</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -862,45 +956,59 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2.417662932527851</t>
-        </is>
-      </c>
-      <c r="G8" t="n">
+          <t>TKD</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>JVVSK94938418</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>2.417662932527851</v>
+      </c>
+      <c r="I8" t="n">
         <v>4</v>
       </c>
-      <c r="H8" t="n">
+      <c r="J8" t="n">
         <v>3</v>
       </c>
-      <c r="I8" t="n">
-        <v>6</v>
-      </c>
-      <c r="J8" t="inlineStr">
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>6.127856803773065</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
         <is>
           <t>7.977021389743102</t>
         </is>
       </c>
-      <c r="K8" t="n">
-        <v>6.872615770719865</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0.4369324131256846</v>
-      </c>
-      <c r="M8" t="n">
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>6.8726157707198645</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>0.43693241312568465</t>
+        </is>
+      </c>
+      <c r="O8" t="n">
         <v>0.6285029833331557</v>
       </c>
-      <c r="N8" t="n">
-        <v>3.229556341470833</v>
-      </c>
-      <c r="O8" t="n">
+      <c r="P8" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q8" t="n">
         <v>4.886337017858914</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>281520012</v>
+        <v>283288652</v>
       </c>
       <c r="B9" t="n">
-        <v>30665364</v>
+        <v>89899705</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -909,53 +1017,67 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>JULIEN</t>
+          <t>Julien</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>3.185339287822264</t>
-        </is>
-      </c>
-      <c r="G9" t="n">
+          <t>WT</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>YJIWP93581095</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>3.185339287822264</v>
+      </c>
+      <c r="I9" t="n">
         <v>5</v>
       </c>
-      <c r="H9" t="n">
+      <c r="J9" t="n">
         <v>4</v>
       </c>
-      <c r="I9" t="n">
-        <v>2</v>
-      </c>
-      <c r="J9" t="inlineStr">
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>2.8034895162903375</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
         <is>
           <t>4.982935225202532</t>
         </is>
       </c>
-      <c r="K9" t="n">
-        <v>2.481547794756681</v>
-      </c>
-      <c r="L9" t="n">
-        <v>3.926905066752112</v>
-      </c>
-      <c r="M9" t="n">
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>2.481547794756681</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>3.926905066752112</t>
+        </is>
+      </c>
+      <c r="O9" t="n">
         <v>6.645483335148143</v>
       </c>
-      <c r="N9" t="n">
-        <v>1.91315705661408</v>
-      </c>
-      <c r="O9" t="n">
+      <c r="P9" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="n">
         <v>2.804991419726441</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>446694816</v>
+        <v>305956210</v>
       </c>
       <c r="B10" t="n">
-        <v>43496057</v>
+        <v>33998282</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -968,49 +1090,63 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>9.640792451783764</t>
-        </is>
-      </c>
-      <c r="G10" t="n">
+          <t>TKD</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>KHTZG58697007</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>9.640792451783764</v>
+      </c>
+      <c r="I10" t="n">
         <v>0</v>
       </c>
-      <c r="H10" t="n">
+      <c r="J10" t="n">
         <v>0</v>
       </c>
-      <c r="I10" t="n">
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>4.521317265740627</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>3.0470772739383536</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>6.220465943861858</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>6.910540612827384</t>
+        </is>
+      </c>
+      <c r="O10" t="n">
+        <v>0.3190525603462713</v>
+      </c>
+      <c r="P10" t="n">
         <v>4</v>
       </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>3.0470772739383536</t>
-        </is>
-      </c>
-      <c r="K10" t="n">
-        <v>6.220465943861858</v>
-      </c>
-      <c r="L10" t="n">
-        <v>6.910540612827384</v>
-      </c>
-      <c r="M10" t="n">
-        <v>0.3190525603462713</v>
-      </c>
-      <c r="N10" t="n">
-        <v>4.968664343329384</v>
-      </c>
-      <c r="O10" t="n">
+      <c r="Q10" t="n">
         <v>8.853302668097649</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>17646726</v>
+        <v>825454272</v>
       </c>
       <c r="B11" t="n">
-        <v>72495953</v>
+        <v>8633742</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -1023,104 +1159,132 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2.6364980427509375</t>
-        </is>
-      </c>
-      <c r="G11" t="n">
+          <t>TKD</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>TXLJM65340594</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>2.636498042750937</v>
+      </c>
+      <c r="I11" t="n">
         <v>2</v>
       </c>
-      <c r="H11" t="n">
+      <c r="J11" t="n">
         <v>2</v>
       </c>
-      <c r="I11" t="n">
-        <v>5</v>
-      </c>
-      <c r="J11" t="inlineStr">
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>5.312210890116851</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
         <is>
           <t>2.342060522066809</t>
         </is>
       </c>
-      <c r="K11" t="n">
-        <v>3.156556907796485</v>
-      </c>
-      <c r="L11" t="n">
-        <v>7.269774313286971</v>
-      </c>
-      <c r="M11" t="n">
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>3.1565569077964852</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>7.269774313286971</t>
+        </is>
+      </c>
+      <c r="O11" t="n">
         <v>2.381556001205146</v>
       </c>
-      <c r="N11" t="n">
-        <v>3.144053207478292</v>
-      </c>
-      <c r="O11" t="n">
+      <c r="P11" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q11" t="n">
         <v>8.07728176625732</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>105712955</v>
+        <v>431564856</v>
       </c>
       <c r="B12" t="n">
-        <v>44959493</v>
+        <v>83977578</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Chevalier (Robert)</t>
+          <t>CHEVALIER (ROBERT)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Isabelle</t>
+          <t>ISABELLE</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>4.410061220535114</t>
-        </is>
-      </c>
-      <c r="G12" t="n">
+          <t>TKD</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>PQOXX59186921</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>4.410061220535114</v>
+      </c>
+      <c r="I12" t="n">
         <v>8</v>
       </c>
-      <c r="H12" t="n">
+      <c r="J12" t="n">
         <v>5</v>
       </c>
-      <c r="I12" t="n">
-        <v>9</v>
-      </c>
-      <c r="J12" t="inlineStr">
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>9.886345634286613</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
         <is>
           <t>8.93008166217633</t>
         </is>
       </c>
-      <c r="K12" t="n">
-        <v>2.772164172083738</v>
-      </c>
-      <c r="L12" t="n">
-        <v>6.690315985377016</v>
-      </c>
-      <c r="M12" t="n">
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>2.7721641720837376</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>6.690315985377016</t>
+        </is>
+      </c>
+      <c r="O12" t="n">
         <v>5.15429653554424</v>
       </c>
-      <c r="N12" t="n">
-        <v>0.3030465846818109</v>
-      </c>
-      <c r="O12" t="n">
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="n">
         <v>4.394491661468117</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>574189981</v>
+        <v>549692660</v>
       </c>
       <c r="B13" t="n">
-        <v>34520600</v>
+        <v>49945932</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -1137,155 +1301,197 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>6.098708094225075</t>
-        </is>
-      </c>
-      <c r="G13" t="n">
+          <t>TKD</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>GFTKF64340259</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>6.098708094225075</v>
+      </c>
+      <c r="I13" t="n">
         <v>4</v>
       </c>
-      <c r="H13" t="n">
+      <c r="J13" t="n">
         <v>7</v>
       </c>
-      <c r="I13" t="n">
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>0.059781688730145</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>3.775365039533037</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>9.298652107952872</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>5.915547336476866</t>
+        </is>
+      </c>
+      <c r="O13" t="n">
+        <v>6.023578195926511</v>
+      </c>
+      <c r="P13" t="n">
         <v>0</v>
       </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>3.775365039533037</t>
-        </is>
-      </c>
-      <c r="K13" t="n">
-        <v>9.298652107952872</v>
-      </c>
-      <c r="L13" t="n">
-        <v>5.915547336476866</v>
-      </c>
-      <c r="M13" t="n">
-        <v>6.023578195926511</v>
-      </c>
-      <c r="N13" t="n">
-        <v>0.9262352470986679</v>
-      </c>
-      <c r="O13" t="n">
+      <c r="Q13" t="n">
         <v>6.416481212367472</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>814479358</v>
+        <v>985836708</v>
       </c>
       <c r="B14" t="n">
-        <v>10959327</v>
+        <v>61113676</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Gauthier</t>
+          <t>GAUTHIER</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Marie-Claire</t>
+          <t>MARIE-CLAIRE</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>8.636212965699608</t>
-        </is>
-      </c>
-      <c r="G14" t="n">
+          <t>TKD</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>QKQIZ66497534</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>8.636212965699608</v>
+      </c>
+      <c r="I14" t="n">
         <v>7</v>
       </c>
-      <c r="H14" t="n">
+      <c r="J14" t="n">
         <v>4</v>
       </c>
-      <c r="I14" t="n">
-        <v>2</v>
-      </c>
-      <c r="J14" t="inlineStr">
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>2.0128828557628275</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
         <is>
           <t>0.7634545162114037</t>
         </is>
       </c>
-      <c r="K14" t="n">
-        <v>2.795952691185541</v>
-      </c>
-      <c r="L14" t="n">
-        <v>8.790005515634675</v>
-      </c>
-      <c r="M14" t="n">
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>2.7959526911855406</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>8.790005515634675</t>
+        </is>
+      </c>
+      <c r="O14" t="n">
         <v>2.829595316807854</v>
       </c>
-      <c r="N14" t="n">
-        <v>5.890203488734043</v>
-      </c>
-      <c r="O14" t="n">
+      <c r="P14" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q14" t="n">
         <v>6.310390607112448</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>288652898</v>
+        <v>924674521</v>
       </c>
       <c r="B15" t="n">
-        <v>99705156</v>
+        <v>73731428</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>BLANC (ROUX)</t>
+          <t>blanc (roux)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>NICOLAS</t>
+          <t>nicolas</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>8.637576707745845</t>
-        </is>
-      </c>
-      <c r="G15" t="n">
+          <t>ITD</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>ZVVCJ08222662</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>8.637576707745845</v>
+      </c>
+      <c r="I15" t="n">
         <v>9</v>
       </c>
-      <c r="H15" t="n">
+      <c r="J15" t="n">
         <v>3</v>
       </c>
-      <c r="I15" t="n">
-        <v>2</v>
-      </c>
-      <c r="J15" t="inlineStr">
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>2.5687579634137636</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
         <is>
           <t>0.3380685443750153</t>
         </is>
       </c>
-      <c r="K15" t="n">
-        <v>9.488350155396008</v>
-      </c>
-      <c r="L15" t="n">
-        <v>5.376576529462347</v>
-      </c>
-      <c r="M15" t="n">
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>9.488350155396008</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>5.376576529462347</t>
+        </is>
+      </c>
+      <c r="O15" t="n">
         <v>8.431300031796804</v>
       </c>
-      <c r="N15" t="n">
-        <v>6.340383820561487</v>
-      </c>
-      <c r="O15" t="n">
+      <c r="P15" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q15" t="n">
         <v>0.08436724109673222</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>586970071</v>
+        <v>667659839</v>
       </c>
       <c r="B16" t="n">
-        <v>46527305</v>
+        <v>99747900</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -1294,7 +1500,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>SOPHIE</t>
+          <t>Sophie</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -1302,45 +1508,59 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>6.748813133496951</t>
-        </is>
-      </c>
-      <c r="G16" t="n">
+          <t>TKD</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>RQEGK96085338</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>6.748813133496951</v>
+      </c>
+      <c r="I16" t="n">
         <v>1</v>
       </c>
-      <c r="H16" t="n">
+      <c r="J16" t="n">
         <v>9</v>
       </c>
-      <c r="I16" t="n">
-        <v>3</v>
-      </c>
-      <c r="J16" t="inlineStr">
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>3.4074483905634736</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
         <is>
           <t>4.616133222332174</t>
         </is>
       </c>
-      <c r="K16" t="n">
-        <v>2.020173512975978</v>
-      </c>
-      <c r="L16" t="n">
-        <v>0.9782239766028444</v>
-      </c>
-      <c r="M16" t="n">
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>2.020173512975978</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>0.9782239766028444</t>
+        </is>
+      </c>
+      <c r="O16" t="n">
         <v>8.947055744396657</v>
       </c>
-      <c r="N16" t="n">
-        <v>9.663444843354702</v>
-      </c>
-      <c r="O16" t="n">
+      <c r="P16" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q16" t="n">
         <v>2.216583474864998</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>339982824</v>
+        <v>248058048</v>
       </c>
       <c r="B17" t="n">
-        <v>9759546</v>
+        <v>670423</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -1357,45 +1577,59 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>6.598743479594312</t>
-        </is>
-      </c>
-      <c r="G17" t="n">
+          <t>TKD</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>MNGBN61622915</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>6.598743479594312</v>
+      </c>
+      <c r="I17" t="n">
         <v>9</v>
       </c>
-      <c r="H17" t="n">
+      <c r="J17" t="n">
         <v>7</v>
       </c>
-      <c r="I17" t="n">
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>0.5300196254547929</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>8.738239607364896</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>5.6547841466236655</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>1.4129582348843794</t>
+        </is>
+      </c>
+      <c r="O17" t="n">
+        <v>7.231912274435535</v>
+      </c>
+      <c r="P17" t="n">
         <v>0</v>
       </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>8.738239607364896</t>
-        </is>
-      </c>
-      <c r="K17" t="n">
-        <v>5.654784146623665</v>
-      </c>
-      <c r="L17" t="n">
-        <v>1.412958234884379</v>
-      </c>
-      <c r="M17" t="n">
-        <v>7.231912274435535</v>
-      </c>
-      <c r="N17" t="n">
-        <v>0.1487968435494547</v>
-      </c>
-      <c r="O17" t="n">
+      <c r="Q17" t="n">
         <v>2.168927834900205</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>594189038</v>
+        <v>626594119</v>
       </c>
       <c r="B18" t="n">
-        <v>99582545</v>
+        <v>69589067</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -1408,49 +1642,63 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>7.357576983159544</t>
-        </is>
-      </c>
-      <c r="G18" t="n">
+          <t>WT</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>OOFIF64804593</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>7.357576983159544</v>
+      </c>
+      <c r="I18" t="n">
         <v>1</v>
       </c>
-      <c r="H18" t="n">
+      <c r="J18" t="n">
         <v>4</v>
       </c>
-      <c r="I18" t="n">
-        <v>3</v>
-      </c>
-      <c r="J18" t="inlineStr">
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>3.2649449538067055</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
         <is>
           <t>3.506094910196108</t>
         </is>
       </c>
-      <c r="K18" t="n">
-        <v>3.803031304256006</v>
-      </c>
-      <c r="L18" t="n">
-        <v>9.622800892721934</v>
-      </c>
-      <c r="M18" t="n">
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>3.803031304256006</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>9.622800892721934</t>
+        </is>
+      </c>
+      <c r="O18" t="n">
         <v>9.26541415360381</v>
       </c>
-      <c r="N18" t="n">
-        <v>7.331599843419532</v>
-      </c>
-      <c r="O18" t="n">
+      <c r="P18" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q18" t="n">
         <v>2.202690277715083</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>863374259</v>
+        <v>509931782</v>
       </c>
       <c r="B19" t="n">
-        <v>68799778</v>
+        <v>90489649</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -1463,58 +1711,72 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2.2275365813138723</t>
-        </is>
-      </c>
-      <c r="G19" t="n">
+          <t>TKD</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>UQDMC58215974</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>2.227536581313872</v>
+      </c>
+      <c r="I19" t="n">
         <v>9</v>
       </c>
-      <c r="H19" t="n">
+      <c r="J19" t="n">
         <v>4</v>
       </c>
-      <c r="I19" t="n">
-        <v>1</v>
-      </c>
-      <c r="J19" t="inlineStr">
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>1.9835820718308184</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
         <is>
           <t>8.235205516449387</t>
         </is>
       </c>
-      <c r="K19" t="n">
-        <v>8.081067272417844</v>
-      </c>
-      <c r="L19" t="n">
-        <v>7.981039042202182</v>
-      </c>
-      <c r="M19" t="n">
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>8.081067272417844</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>7.981039042202182</t>
+        </is>
+      </c>
+      <c r="O19" t="n">
         <v>0.5899723480765795</v>
       </c>
-      <c r="N19" t="n">
-        <v>6.328628553985399</v>
-      </c>
-      <c r="O19" t="n">
+      <c r="P19" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q19" t="n">
         <v>7.41137213731608</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>177188243</v>
+        <v>713155565</v>
       </c>
       <c r="B20" t="n">
-        <v>15648568</v>
+        <v>10227521</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>GAGNON_LAVOIE</t>
+          <t>Gagnon_Lavoie</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>ÉMILIE</t>
+          <t>Émilie</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -1522,54 +1784,68 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>1.7206618466113854</t>
-        </is>
-      </c>
-      <c r="G20" t="n">
+          <t>WT</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>CQYHD40110489</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>1.720661846611385</v>
+      </c>
+      <c r="I20" t="n">
         <v>0</v>
       </c>
-      <c r="H20" t="n">
+      <c r="J20" t="n">
         <v>7</v>
       </c>
-      <c r="I20" t="n">
-        <v>8</v>
-      </c>
-      <c r="J20" t="inlineStr">
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>8.292149093742202</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
         <is>
           <t>9.471990743671517</t>
         </is>
       </c>
-      <c r="K20" t="n">
-        <v>1.275536679476561</v>
-      </c>
-      <c r="L20" t="n">
-        <v>0.06753772081126819</v>
-      </c>
-      <c r="M20" t="n">
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>1.275536679476561</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>0.06753772081126819</t>
+        </is>
+      </c>
+      <c r="O20" t="n">
         <v>0.5014746330699005</v>
       </c>
-      <c r="N20" t="n">
-        <v>5.016849210767741</v>
-      </c>
-      <c r="O20" t="n">
+      <c r="P20" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q20" t="n">
         <v>9.415540094377699</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>818711329</v>
+        <v>672687964</v>
       </c>
       <c r="B21" t="n">
-        <v>52643402</v>
+        <v>94425249</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Côté (Bouchard)</t>
+          <t>CÔTÉ (BOUCHARD)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Marc</t>
+          <t>MARC</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -1577,36 +1853,50 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>8.704149724889355</t>
-        </is>
-      </c>
-      <c r="G21" t="n">
+          <t>ITD</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>RTPTC86506538</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>8.704149724889355</v>
+      </c>
+      <c r="I21" t="n">
         <v>4</v>
       </c>
-      <c r="H21" t="n">
+      <c r="J21" t="n">
         <v>8</v>
       </c>
-      <c r="I21" t="n">
-        <v>6</v>
-      </c>
-      <c r="J21" t="inlineStr">
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>6.371216286308995</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
         <is>
           <t>0.6704070988991806</t>
         </is>
       </c>
-      <c r="K21" t="n">
-        <v>9.513395513366476</v>
-      </c>
-      <c r="L21" t="n">
-        <v>9.458115437886523</v>
-      </c>
-      <c r="M21" t="n">
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>9.513395513366476</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>9.458115437886523</t>
+        </is>
+      </c>
+      <c r="O21" t="n">
         <v>1.238801221829032</v>
       </c>
-      <c r="N21" t="n">
-        <v>1.209365536809416</v>
-      </c>
-      <c r="O21" t="n">
+      <c r="P21" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q21" t="n">
         <v>2.664372993571338</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tune column white list
</commit_message>
<xml_diff>
--- a/mock_metadata.xlsx
+++ b/mock_metadata.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,55 +466,60 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>NPM</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>mock_col_0</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>mock_col_1</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>mock_col_2</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>mock_col_3</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>mock_col_4</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>mock_col_5</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>mock_col_6</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>mock_col_7</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>mock_col_8</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>mock_col_9</t>
         </is>
@@ -547,54 +552,61 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
+          <t>NPM type A</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
           <t>CZSBV11530005</t>
         </is>
       </c>
-      <c r="H2" t="n">
-        <v>9.766997666981421</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>9.766997666981421</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>0.6013865780151506</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
         <v>8</v>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>2.935015581362097</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>0.8544073566273735</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>2.9784009061862315</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>7.288273572721245</t>
-        </is>
-      </c>
       <c r="O2" t="n">
+        <v>7.288273572721245</v>
+      </c>
+      <c r="P2" t="n">
         <v>6.554225855557608</v>
       </c>
-      <c r="P2" t="n">
+      <c r="Q2" t="n">
         <v>1</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="R2" t="n">
         <v>8.579403861447053</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>183205182</v>
+        <v>205182470</v>
       </c>
       <c r="B3" t="n">
-        <v>47064024</v>
+        <v>64024242</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -607,63 +619,70 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>ITD</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>UGOQV08105276</t>
-        </is>
-      </c>
-      <c r="H3" t="n">
-        <v>3.801957350196178</v>
-      </c>
-      <c r="I3" t="n">
-        <v>6</v>
-      </c>
-      <c r="J3" t="n">
+          <t>NPM type D</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>OQVAQ10527620</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>3.8019573501961776</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>6.836889090860106</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
         <v>2</v>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>7.333144993171773</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>2.2016043728738346</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>6.19161016367253</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>1.7554499781764055</t>
-        </is>
-      </c>
       <c r="O3" t="n">
+        <v>1.755449978176405</v>
+      </c>
+      <c r="P3" t="n">
         <v>9.106845690724835</v>
       </c>
-      <c r="P3" t="n">
+      <c r="Q3" t="n">
         <v>5</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="R3" t="n">
         <v>7.024108748899226</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>266181764</v>
+        <v>764351294</v>
       </c>
       <c r="B4" t="n">
-        <v>35129425</v>
+        <v>25711630</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -680,68 +699,75 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>TKD</t>
+          <t>ITD</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>SMYLP59770792</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>9.232462337639554</v>
-      </c>
-      <c r="I4" t="n">
-        <v>6</v>
-      </c>
-      <c r="J4" t="n">
+          <t>NF</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>SOPBZ79278744</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>9.232462337639554</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>6.712380191408013</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
         <v>8</v>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>8.088307025622912</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>6.8117600564649585</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="N4" t="inlineStr">
         <is>
           <t>3.017574296201845</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>6.9275909358149566</t>
-        </is>
-      </c>
       <c r="O4" t="n">
+        <v>6.927590935814957</v>
+      </c>
+      <c r="P4" t="n">
         <v>1.525846598449274</v>
       </c>
-      <c r="P4" t="n">
+      <c r="Q4" t="n">
         <v>9</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="R4" t="n">
         <v>5.686140286219992</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>378353862</v>
+        <v>405827875</v>
       </c>
       <c r="B5" t="n">
-        <v>93405827</v>
+        <v>22092281</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Durand (Thomas)</t>
+          <t>DURAND (THOMAS)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Claire</t>
+          <t>CLAIRE</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -749,68 +775,75 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>ITD</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>GBJZB38154719</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
-        <v>2.616924238635442</v>
-      </c>
-      <c r="I5" t="n">
-        <v>6</v>
-      </c>
-      <c r="J5" t="n">
+          <t>neg</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>OCSIC63163783</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2.616924238635442</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>6.110179811110102</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
         <v>9</v>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>8.870869741717364</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>1.3441008942863109</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
+      <c r="N5" t="inlineStr">
         <is>
           <t>1.7484645112507746</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>0.9283302374194224</t>
-        </is>
-      </c>
       <c r="O5" t="n">
+        <v>0.9283302374194224</v>
+      </c>
+      <c r="P5" t="n">
         <v>5.886323190849075</v>
       </c>
-      <c r="P5" t="n">
+      <c r="Q5" t="n">
         <v>1</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="R5" t="n">
         <v>9.810992114290196</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>846592814</v>
+        <v>694816434</v>
       </c>
       <c r="B6" t="n">
-        <v>46694816</v>
+        <v>96057372</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>petit</t>
+          <t>Petit</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>lucas</t>
+          <t>Lucas</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -818,68 +851,75 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>ITD</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>TFERC52001230</t>
-        </is>
-      </c>
-      <c r="H6" t="n">
-        <v>3.190970584141976</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="n">
+          <t>neg</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>GBNMX53648465</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>3.1909705841419758</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>0.6013731275422918</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
         <v>8</v>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>0.24833211267027866</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
+      <c r="M6" t="inlineStr">
         <is>
           <t>9.565136908680433</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
+      <c r="N6" t="inlineStr">
         <is>
           <t>4.95505195217647</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>5.564015705845731</t>
-        </is>
-      </c>
       <c r="O6" t="n">
+        <v>5.564015705845731</v>
+      </c>
+      <c r="P6" t="n">
         <v>5.037655996150194</v>
       </c>
-      <c r="P6" t="n">
+      <c r="Q6" t="n">
         <v>9</v>
       </c>
-      <c r="Q6" t="n">
+      <c r="R6" t="n">
         <v>0.9035270116837701</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>495953289</v>
+        <v>71057129</v>
       </c>
       <c r="B7" t="n">
-        <v>77071057</v>
+        <v>55449594</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>DUBOIS_MARTIN</t>
+          <t>Dubois_Martin</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>PAUL</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -887,63 +927,70 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>ITD</t>
+          <t>TKD</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>LOHYP26401764</t>
-        </is>
-      </c>
-      <c r="H7" t="n">
-        <v>1.180912329666428</v>
-      </c>
-      <c r="I7" t="n">
-        <v>9</v>
-      </c>
-      <c r="J7" t="n">
+          <t>NPM type A</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>JNVPF67249595</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>1.1809123296664281</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>9.777692736076393</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
         <v>4</v>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="L7" t="inlineStr">
         <is>
           <t>5.125494476917045</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
+      <c r="M7" t="inlineStr">
         <is>
           <t>1.3652397740514988</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
+      <c r="N7" t="inlineStr">
         <is>
           <t>7.605704002660505</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>1.024941347304994</t>
-        </is>
-      </c>
       <c r="O7" t="n">
+        <v>1.024941347304994</v>
+      </c>
+      <c r="P7" t="n">
         <v>1.738089819802944</v>
       </c>
-      <c r="P7" t="n">
+      <c r="Q7" t="n">
         <v>8</v>
       </c>
-      <c r="Q7" t="n">
+      <c r="R7" t="n">
         <v>7.270797710217943</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>418998134</v>
+        <v>325856814</v>
       </c>
       <c r="B8" t="n">
-        <v>52060032</v>
+        <v>47935810</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Moreau</t>
+          <t>MOREAU</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -961,58 +1008,65 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>JVVSK94938418</t>
-        </is>
-      </c>
-      <c r="H8" t="n">
-        <v>2.417662932527851</v>
-      </c>
-      <c r="I8" t="n">
-        <v>4</v>
-      </c>
-      <c r="J8" t="n">
+          <t>NF</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>QKKOI18998134</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>2.417662932527851</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>4.38951626746782</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
         <v>3</v>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="L8" t="inlineStr">
         <is>
           <t>6.127856803773065</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
+      <c r="M8" t="inlineStr">
         <is>
           <t>7.977021389743102</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
+      <c r="N8" t="inlineStr">
         <is>
           <t>6.8726157707198645</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>0.43693241312568465</t>
-        </is>
-      </c>
       <c r="O8" t="n">
+        <v>0.4369324131256846</v>
+      </c>
+      <c r="P8" t="n">
         <v>0.6285029833331557</v>
       </c>
-      <c r="P8" t="n">
+      <c r="Q8" t="n">
         <v>3</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="R8" t="n">
         <v>4.886337017858914</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>283288652</v>
+        <v>51560991</v>
       </c>
       <c r="B9" t="n">
-        <v>89899705</v>
+        <v>53935869</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>LAURENT_GIRARD</t>
+          <t>Laurent_Girard</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1021,72 +1075,79 @@
         </is>
       </c>
       <c r="E9" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>ITD</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>neg</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>VVERT91283288</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>3.185339287822264</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>5.325950215229039</t>
+        </is>
+      </c>
+      <c r="K9" t="n">
+        <v>4</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>2.8034895162903375</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>4.982935225202532</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>2.481547794756681</t>
+        </is>
+      </c>
+      <c r="O9" t="n">
+        <v>3.926905066752112</v>
+      </c>
+      <c r="P9" t="n">
+        <v>6.645483335148143</v>
+      </c>
+      <c r="Q9" t="n">
         <v>1</v>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>WT</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>YJIWP93581095</t>
-        </is>
-      </c>
-      <c r="H9" t="n">
-        <v>3.185339287822264</v>
-      </c>
-      <c r="I9" t="n">
-        <v>5</v>
-      </c>
-      <c r="J9" t="n">
-        <v>4</v>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>2.8034895162903375</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>4.982935225202532</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>2.481547794756681</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>3.926905066752112</t>
-        </is>
-      </c>
-      <c r="O9" t="n">
-        <v>6.645483335148143</v>
-      </c>
-      <c r="P9" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q9" t="n">
+      <c r="R9" t="n">
         <v>2.804991419726441</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>305956210</v>
+        <v>824097595</v>
       </c>
       <c r="B10" t="n">
-        <v>33998282</v>
+        <v>46653405</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Simon (Dupuis)</t>
+          <t>SIMON (DUPUIS)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Emma</t>
+          <t>EMMA</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -1094,68 +1155,75 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>TKD</t>
+          <t>ITD</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>KHTZG58697007</t>
-        </is>
-      </c>
-      <c r="H10" t="n">
-        <v>9.640792451783764</v>
-      </c>
-      <c r="I10" t="n">
+          <t>neg</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>NKEPV30595621</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>9.640792451783764</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>0.031322874578293414</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
         <v>0</v>
       </c>
-      <c r="J10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" t="inlineStr">
+      <c r="L10" t="inlineStr">
         <is>
           <t>4.521317265740627</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="M10" t="inlineStr">
         <is>
           <t>3.0470772739383536</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr">
+      <c r="N10" t="inlineStr">
         <is>
           <t>6.220465943861858</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>6.910540612827384</t>
-        </is>
-      </c>
       <c r="O10" t="n">
+        <v>6.910540612827384</v>
+      </c>
+      <c r="P10" t="n">
         <v>0.3190525603462713</v>
       </c>
-      <c r="P10" t="n">
+      <c r="Q10" t="n">
         <v>4</v>
       </c>
-      <c r="Q10" t="n">
+      <c r="R10" t="n">
         <v>8.853302668097649</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>825454272</v>
+        <v>879977875</v>
       </c>
       <c r="B11" t="n">
-        <v>8633742</v>
+        <v>91869217</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>lefèvre_rousseau</t>
+          <t>Lefèvre_Rousseau</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>léa</t>
+          <t>Léa</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -1163,137 +1231,151 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>TKD</t>
+          <t>ITD</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>TXLJM65340594</t>
-        </is>
-      </c>
-      <c r="H11" t="n">
-        <v>2.636498042750937</v>
-      </c>
-      <c r="I11" t="n">
+          <t>NF</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>KJLIW27208633</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>2.6364980427509375</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>2.5126710549130427</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
         <v>2</v>
       </c>
-      <c r="J11" t="n">
-        <v>2</v>
-      </c>
-      <c r="K11" t="inlineStr">
+      <c r="L11" t="inlineStr">
         <is>
           <t>5.312210890116851</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr">
+      <c r="M11" t="inlineStr">
         <is>
           <t>2.342060522066809</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr">
+      <c r="N11" t="inlineStr">
         <is>
           <t>3.1565569077964852</t>
         </is>
       </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>7.269774313286971</t>
-        </is>
-      </c>
       <c r="O11" t="n">
+        <v>7.269774313286971</v>
+      </c>
+      <c r="P11" t="n">
         <v>2.381556001205146</v>
       </c>
-      <c r="P11" t="n">
+      <c r="Q11" t="n">
         <v>3</v>
       </c>
-      <c r="Q11" t="n">
+      <c r="R11" t="n">
         <v>8.07728176625732</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>431564856</v>
+        <v>132952643</v>
       </c>
       <c r="B12" t="n">
-        <v>83977578</v>
+        <v>40259100</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CHEVALIER (ROBERT)</t>
+          <t>Chevalier (Robert)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>ISABELLE</t>
+          <t>Isabelle</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>TKD</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>PQOXX59186921</t>
-        </is>
-      </c>
-      <c r="H12" t="n">
-        <v>4.410061220535114</v>
-      </c>
-      <c r="I12" t="n">
-        <v>8</v>
-      </c>
-      <c r="J12" t="n">
+          <t>NPM type A</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>KMJWQ56839775</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>4.410061220535114</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>8.584904374223306</t>
+        </is>
+      </c>
+      <c r="K12" t="n">
         <v>5</v>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="L12" t="inlineStr">
         <is>
           <t>9.886345634286613</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr">
+      <c r="M12" t="inlineStr">
         <is>
           <t>8.93008166217633</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr">
+      <c r="N12" t="inlineStr">
         <is>
           <t>2.7721641720837376</t>
         </is>
       </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>6.690315985377016</t>
-        </is>
-      </c>
       <c r="O12" t="n">
+        <v>6.690315985377016</v>
+      </c>
+      <c r="P12" t="n">
         <v>5.15429653554424</v>
       </c>
-      <c r="P12" t="n">
+      <c r="Q12" t="n">
         <v>0</v>
       </c>
-      <c r="Q12" t="n">
+      <c r="R12" t="n">
         <v>4.394491661468117</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>549692660</v>
+        <v>685846649</v>
       </c>
       <c r="B13" t="n">
-        <v>49945932</v>
+        <v>75342262</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>mercier_lemoine</t>
+          <t>Mercier_Lemoine</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>antoine</t>
+          <t>Antoine</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -1301,137 +1383,151 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>TKD</t>
+          <t>ITD</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>GFTKF64340259</t>
-        </is>
-      </c>
-      <c r="H13" t="n">
-        <v>6.098708094225075</v>
-      </c>
-      <c r="I13" t="n">
-        <v>4</v>
-      </c>
-      <c r="J13" t="n">
+          <t>NPM type A</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>WSVFM60499459</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>6.098708094225075</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>4.252983511963176</t>
+        </is>
+      </c>
+      <c r="K13" t="n">
         <v>7</v>
       </c>
-      <c r="K13" t="inlineStr">
+      <c r="L13" t="inlineStr">
         <is>
           <t>0.059781688730145</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr">
+      <c r="M13" t="inlineStr">
         <is>
           <t>3.775365039533037</t>
         </is>
       </c>
-      <c r="M13" t="inlineStr">
+      <c r="N13" t="inlineStr">
         <is>
           <t>9.298652107952872</t>
         </is>
       </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>5.915547336476866</t>
-        </is>
-      </c>
       <c r="O13" t="n">
+        <v>5.915547336476866</v>
+      </c>
+      <c r="P13" t="n">
         <v>6.023578195926511</v>
       </c>
-      <c r="P13" t="n">
+      <c r="Q13" t="n">
         <v>0</v>
       </c>
-      <c r="Q13" t="n">
+      <c r="R13" t="n">
         <v>6.416481212367472</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>985836708</v>
+        <v>82226628</v>
       </c>
       <c r="B14" t="n">
-        <v>61113676</v>
+        <v>24178592</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>GAUTHIER</t>
+          <t>gauthier</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>MARIE-CLAIRE</t>
+          <t>marie-claire</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>TKD</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>QKQIZ66497534</t>
-        </is>
-      </c>
-      <c r="H14" t="n">
-        <v>8.636212965699608</v>
-      </c>
-      <c r="I14" t="n">
-        <v>7</v>
-      </c>
-      <c r="J14" t="n">
+          <t>NPM type D</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>ARMYC11367634</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>8.636212965699608</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>7.358189940396671</t>
+        </is>
+      </c>
+      <c r="K14" t="n">
         <v>4</v>
       </c>
-      <c r="K14" t="inlineStr">
+      <c r="L14" t="inlineStr">
         <is>
           <t>2.0128828557628275</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr">
+      <c r="M14" t="inlineStr">
         <is>
           <t>0.7634545162114037</t>
         </is>
       </c>
-      <c r="M14" t="inlineStr">
+      <c r="N14" t="inlineStr">
         <is>
           <t>2.7959526911855406</t>
         </is>
       </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>8.790005515634675</t>
-        </is>
-      </c>
       <c r="O14" t="n">
+        <v>8.790005515634675</v>
+      </c>
+      <c r="P14" t="n">
         <v>2.829595316807854</v>
       </c>
-      <c r="P14" t="n">
+      <c r="Q14" t="n">
         <v>5</v>
       </c>
-      <c r="Q14" t="n">
+      <c r="R14" t="n">
         <v>6.310390607112448</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>924674521</v>
+        <v>596085338</v>
       </c>
       <c r="B15" t="n">
-        <v>73731428</v>
+        <v>573066</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>blanc (roux)</t>
+          <t>BLANC (ROUX)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>nicolas</t>
+          <t>NICOLAS</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -1439,59 +1535,66 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>ITD</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>ZVVCJ08222662</t>
-        </is>
-      </c>
-      <c r="H15" t="n">
-        <v>8.637576707745845</v>
-      </c>
-      <c r="I15" t="n">
-        <v>9</v>
-      </c>
-      <c r="J15" t="n">
+          <t>NPM type A</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>CZOHO31428426</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>8.637576707745845</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>9.220432168103056</t>
+        </is>
+      </c>
+      <c r="K15" t="n">
         <v>3</v>
       </c>
-      <c r="K15" t="inlineStr">
+      <c r="L15" t="inlineStr">
         <is>
           <t>2.5687579634137636</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr">
+      <c r="M15" t="inlineStr">
         <is>
           <t>0.3380685443750153</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr">
+      <c r="N15" t="inlineStr">
         <is>
           <t>9.488350155396008</t>
         </is>
       </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>5.376576529462347</t>
-        </is>
-      </c>
       <c r="O15" t="n">
+        <v>5.376576529462347</v>
+      </c>
+      <c r="P15" t="n">
         <v>8.431300031796804</v>
       </c>
-      <c r="P15" t="n">
+      <c r="Q15" t="n">
         <v>6</v>
       </c>
-      <c r="Q15" t="n">
+      <c r="R15" t="n">
         <v>0.08436724109673222</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>667659839</v>
+        <v>291523186</v>
       </c>
       <c r="B16" t="n">
-        <v>99747900</v>
+        <v>2480580</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -1500,7 +1603,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Sophie</t>
+          <t>SOPHIE</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -1513,63 +1616,70 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>RQEGK96085338</t>
-        </is>
-      </c>
-      <c r="H16" t="n">
-        <v>6.748813133496951</v>
-      </c>
-      <c r="I16" t="n">
-        <v>1</v>
-      </c>
-      <c r="J16" t="n">
+          <t>neg</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>PSAAJ91793663</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>6.748813133496951</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>1.5347417112811557</t>
+        </is>
+      </c>
+      <c r="K16" t="n">
         <v>9</v>
       </c>
-      <c r="K16" t="inlineStr">
+      <c r="L16" t="inlineStr">
         <is>
           <t>3.4074483905634736</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr">
+      <c r="M16" t="inlineStr">
         <is>
           <t>4.616133222332174</t>
         </is>
       </c>
-      <c r="M16" t="inlineStr">
+      <c r="N16" t="inlineStr">
         <is>
           <t>2.020173512975978</t>
         </is>
       </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>0.9782239766028444</t>
-        </is>
-      </c>
       <c r="O16" t="n">
+        <v>0.9782239766028444</v>
+      </c>
+      <c r="P16" t="n">
         <v>8.947055744396657</v>
       </c>
-      <c r="P16" t="n">
+      <c r="Q16" t="n">
         <v>9</v>
       </c>
-      <c r="Q16" t="n">
+      <c r="R16" t="n">
         <v>2.216583474864998</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>248058048</v>
+        <v>804593204</v>
       </c>
       <c r="B17" t="n">
-        <v>670423</v>
+        <v>97062659</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Roy (Leroy)</t>
+          <t>roy (leroy)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Juliette</t>
+          <t>juliette</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -1577,68 +1687,75 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>TKD</t>
+          <t>ITD</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>MNGBN61622915</t>
-        </is>
-      </c>
-      <c r="H17" t="n">
-        <v>6.598743479594312</v>
-      </c>
-      <c r="I17" t="n">
-        <v>9</v>
-      </c>
-      <c r="J17" t="n">
+          <t>neg</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>AWYJF39790437</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>6.598743479594312</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>9.92259229487619</t>
+        </is>
+      </c>
+      <c r="K17" t="n">
         <v>7</v>
       </c>
-      <c r="K17" t="inlineStr">
+      <c r="L17" t="inlineStr">
         <is>
           <t>0.5300196254547929</t>
         </is>
       </c>
-      <c r="L17" t="inlineStr">
+      <c r="M17" t="inlineStr">
         <is>
           <t>8.738239607364896</t>
         </is>
       </c>
-      <c r="M17" t="inlineStr">
+      <c r="N17" t="inlineStr">
         <is>
           <t>5.6547841466236655</t>
         </is>
       </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>1.4129582348843794</t>
-        </is>
-      </c>
       <c r="O17" t="n">
+        <v>1.412958234884379</v>
+      </c>
+      <c r="P17" t="n">
         <v>7.231912274435535</v>
       </c>
-      <c r="P17" t="n">
+      <c r="Q17" t="n">
         <v>0</v>
       </c>
-      <c r="Q17" t="n">
+      <c r="R17" t="n">
         <v>2.168927834900205</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>626594119</v>
+        <v>821597411</v>
       </c>
       <c r="B18" t="n">
-        <v>69589067</v>
+        <v>97905099</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>FONTAINE_MICHEL</t>
+          <t>fontaine_michel</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Vincent</t>
+          <t>vincent</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -1646,72 +1763,79 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>ITD</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>OOFIF64804593</t>
-        </is>
-      </c>
-      <c r="H18" t="n">
-        <v>7.357576983159544</v>
-      </c>
-      <c r="I18" t="n">
-        <v>1</v>
-      </c>
-      <c r="J18" t="n">
+          <t>NPM type D</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>VZNOQ26188598</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>7.357576983159544</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>1.8233178284895335</t>
+        </is>
+      </c>
+      <c r="K18" t="n">
         <v>4</v>
       </c>
-      <c r="K18" t="inlineStr">
+      <c r="L18" t="inlineStr">
         <is>
           <t>3.2649449538067055</t>
         </is>
       </c>
-      <c r="L18" t="inlineStr">
+      <c r="M18" t="inlineStr">
         <is>
           <t>3.506094910196108</t>
         </is>
       </c>
-      <c r="M18" t="inlineStr">
+      <c r="N18" t="inlineStr">
         <is>
           <t>3.803031304256006</t>
         </is>
       </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>9.622800892721934</t>
-        </is>
-      </c>
       <c r="O18" t="n">
+        <v>9.622800892721934</v>
+      </c>
+      <c r="P18" t="n">
         <v>9.26541415360381</v>
       </c>
-      <c r="P18" t="n">
+      <c r="Q18" t="n">
         <v>7</v>
       </c>
-      <c r="Q18" t="n">
+      <c r="R18" t="n">
         <v>2.202690277715083</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>509931782</v>
+        <v>11048959</v>
       </c>
       <c r="B19" t="n">
-        <v>90489649</v>
+        <v>69067131</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Morin (Gagnon)</t>
+          <t>morin (gagnon)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>charlotte</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1720,54 +1844,61 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>UQDMC58215974</t>
-        </is>
-      </c>
-      <c r="H19" t="n">
-        <v>2.227536581313872</v>
-      </c>
-      <c r="I19" t="n">
-        <v>9</v>
-      </c>
-      <c r="J19" t="n">
+          <t>NPM type A</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>QVYSM49909585</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>2.2275365813138723</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>9.401129022827245</t>
+        </is>
+      </c>
+      <c r="K19" t="n">
         <v>4</v>
       </c>
-      <c r="K19" t="inlineStr">
+      <c r="L19" t="inlineStr">
         <is>
           <t>1.9835820718308184</t>
         </is>
       </c>
-      <c r="L19" t="inlineStr">
+      <c r="M19" t="inlineStr">
         <is>
           <t>8.235205516449387</t>
         </is>
       </c>
-      <c r="M19" t="inlineStr">
+      <c r="N19" t="inlineStr">
         <is>
           <t>8.081067272417844</t>
         </is>
       </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>7.981039042202182</t>
-        </is>
-      </c>
       <c r="O19" t="n">
+        <v>7.981039042202182</v>
+      </c>
+      <c r="P19" t="n">
         <v>0.5899723480765795</v>
       </c>
-      <c r="P19" t="n">
+      <c r="Q19" t="n">
         <v>6</v>
       </c>
-      <c r="Q19" t="n">
+      <c r="R19" t="n">
         <v>7.41137213731608</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>713155565</v>
+        <v>918650653</v>
       </c>
       <c r="B20" t="n">
-        <v>10227521</v>
+        <v>82993626</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -1780,72 +1911,79 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>TKD</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>CQYHD40110489</t>
-        </is>
-      </c>
-      <c r="H20" t="n">
-        <v>1.720661846611385</v>
-      </c>
-      <c r="I20" t="n">
-        <v>0</v>
-      </c>
-      <c r="J20" t="n">
+          <t>NF</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>WDAEE75210492</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>1.7206618466113854</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>0.868830552731864</t>
+        </is>
+      </c>
+      <c r="K20" t="n">
         <v>7</v>
       </c>
-      <c r="K20" t="inlineStr">
+      <c r="L20" t="inlineStr">
         <is>
           <t>8.292149093742202</t>
         </is>
       </c>
-      <c r="L20" t="inlineStr">
+      <c r="M20" t="inlineStr">
         <is>
           <t>9.471990743671517</t>
         </is>
       </c>
-      <c r="M20" t="inlineStr">
+      <c r="N20" t="inlineStr">
         <is>
           <t>1.275536679476561</t>
         </is>
       </c>
-      <c r="N20" t="inlineStr">
-        <is>
-          <t>0.06753772081126819</t>
-        </is>
-      </c>
       <c r="O20" t="n">
+        <v>0.06753772081126819</v>
+      </c>
+      <c r="P20" t="n">
         <v>0.5014746330699005</v>
       </c>
-      <c r="P20" t="n">
+      <c r="Q20" t="n">
         <v>5</v>
       </c>
-      <c r="Q20" t="n">
+      <c r="R20" t="n">
         <v>9.415540094377699</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>672687964</v>
+        <v>650508039</v>
       </c>
       <c r="B21" t="n">
-        <v>94425249</v>
+        <v>43764586</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>CÔTÉ (BOUCHARD)</t>
+          <t>côté (bouchard)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>MARC</t>
+          <t>marc</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -1853,50 +1991,57 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>ITD</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>RTPTC86506538</t>
-        </is>
-      </c>
-      <c r="H21" t="n">
-        <v>8.704149724889355</v>
-      </c>
-      <c r="I21" t="n">
-        <v>4</v>
-      </c>
-      <c r="J21" t="n">
+          <t>NPM type D</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>JSIIE52494342</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>8.704149724889355</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>4.682107150738509</t>
+        </is>
+      </c>
+      <c r="K21" t="n">
         <v>8</v>
       </c>
-      <c r="K21" t="inlineStr">
+      <c r="L21" t="inlineStr">
         <is>
           <t>6.371216286308995</t>
         </is>
       </c>
-      <c r="L21" t="inlineStr">
+      <c r="M21" t="inlineStr">
         <is>
           <t>0.6704070988991806</t>
         </is>
       </c>
-      <c r="M21" t="inlineStr">
+      <c r="N21" t="inlineStr">
         <is>
           <t>9.513395513366476</t>
         </is>
       </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>9.458115437886523</t>
-        </is>
-      </c>
       <c r="O21" t="n">
+        <v>9.458115437886523</v>
+      </c>
+      <c r="P21" t="n">
         <v>1.238801221829032</v>
       </c>
-      <c r="P21" t="n">
+      <c r="Q21" t="n">
         <v>1</v>
       </c>
-      <c r="Q21" t="n">
+      <c r="R21" t="n">
         <v>2.664372993571338</v>
       </c>
     </row>

</xml_diff>